<commit_message>
code and figures for microfluidic AI
</commit_message>
<xml_diff>
--- a/Tables/NNs_per_application/3_count_per_application_and_year.xlsx
+++ b/Tables/NNs_per_application/3_count_per_application_and_year.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C8" t="n">
         <v>4</v>
@@ -544,40 +544,40 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dataset generation</t>
+          <t>Bio-implementation</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2017</v>
+        <v>2023</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dataset generation</t>
+          <t>Bio-implementation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dataset generation</t>
+          <t>Bio-implementation</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2020</v>
+        <v>2004</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2021</v>
+        <v>2005</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2022</v>
+        <v>2010</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2023</v>
+        <v>2011</v>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2024</v>
+        <v>2012</v>
       </c>
       <c r="C16" t="n">
         <v>2</v>
@@ -648,37 +648,37 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Explainability</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Explainability</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Explainability</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2024</v>
+        <v>2016</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -687,24 +687,24 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MAC layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
@@ -713,131 +713,300 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C22" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Dataset generation</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PHY layer</t>
+          <t>Explainability</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Upper layers</t>
+          <t>Explainability</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2017</v>
+        <v>2023</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Upper layers</t>
+          <t>Explainability</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Explainability</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>MAC layer</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C34" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C37" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C38" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C39" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PHY layer</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>Upper layers</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B42" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Upper layers</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Upper layers</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>2024</v>
       </c>
-      <c r="C31" t="n">
-        <v>1</v>
+      <c r="C44" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>